<commit_message>
Added control char support to optimized strings.
</commit_message>
<xml_diff>
--- a/test/functional/xlsx_files/shared_strings01.xlsx
+++ b/test/functional/xlsx_files/shared_strings01.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+  <si>
+    <t>_x0000_</t>
+  </si>
   <si>
     <t>_x0001_</t>
   </si>
@@ -721,635 +724,640 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A127"/>
+  <dimension ref="A1:A127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>